<commit_message>
Desenvolvimento de Análise Primária sobre o projeto
Adicionado documentos e explicações sobre a forma que o sistema irá se
comportar.
</commit_message>
<xml_diff>
--- a/Programa/Documentos/1-Análise Primária/Entidades.xlsx
+++ b/Programa/Documentos/1-Análise Primária/Entidades.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
+    <sheet name="Pessoa" sheetId="2" r:id="rId2"/>
+    <sheet name="Refeição" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>Nome</t>
   </si>
@@ -64,14 +64,169 @@
   </si>
   <si>
     <t>Legumes</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Nulo?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Nome do alimento</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Carbohydrates</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>1.000 g</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carboidratos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteínas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gorduras </t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gênero </t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>Frutas, Legumes, Verduras, Carnes, dentre outros</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>Int16</t>
+  </si>
+  <si>
+    <t>SexualGender</t>
+  </si>
+  <si>
+    <t>Gênero Sexual</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Registro do Vigilantes do Peso</t>
+  </si>
+  <si>
+    <t>Campos a se pensar:</t>
+  </si>
+  <si>
+    <t>Peso objetivado</t>
+  </si>
+  <si>
+    <t>Pontos por dia</t>
+  </si>
+  <si>
+    <t>Pontos extras por semana</t>
+  </si>
+  <si>
+    <t>EnergyValue</t>
+  </si>
+  <si>
+    <t>Valor Energético</t>
+  </si>
+  <si>
+    <t>Tipo Refeição</t>
+  </si>
+  <si>
+    <t>Alimentos</t>
+  </si>
+  <si>
+    <t>Pontos totais</t>
+  </si>
+  <si>
+    <t>Cálculo obtido através dos alimentos registrados no BD</t>
+  </si>
+  <si>
+    <t>São até 6 refeições por dia: Café da manhã, Lanche manhã, Almoço, Lanche Tarde, Café da tarde, Jantar</t>
+  </si>
+  <si>
+    <t>Alimentos consumidos na refeição</t>
+  </si>
+  <si>
+    <t>Alimentos[]</t>
+  </si>
+  <si>
+    <t>String[]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -95,12 +250,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,161 +673,1014 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:I8"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="11" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9">
-      <c r="B4" t="s">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="T2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="U2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="V2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="W2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="X2" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="Y2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" t="s">
+    <row r="3" spans="1:25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="S3">
         <v>22</v>
       </c>
-      <c r="D5">
+      <c r="T3">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="U3">
         <v>1.3</v>
       </c>
-      <c r="F5">
+      <c r="V3">
         <v>2.6</v>
       </c>
-      <c r="G5">
+      <c r="W3">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="X3">
         <v>19</v>
       </c>
-      <c r="I5" t="s">
+      <c r="Y3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" t="s">
+    <row r="4" spans="1:25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="Y4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" t="s">
+    <row r="5" spans="1:25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="S5">
         <v>100</v>
       </c>
-      <c r="D7">
+      <c r="T5">
         <v>100</v>
       </c>
-      <c r="E7">
+      <c r="U5">
         <v>100</v>
       </c>
-      <c r="F7">
+      <c r="V5">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="W5">
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="X5">
         <v>100</v>
       </c>
-      <c r="I7" t="s">
+      <c r="Y5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" t="s">
+    <row r="6" spans="1:25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="S6">
         <v>100</v>
       </c>
-      <c r="D8">
+      <c r="T6">
         <v>100</v>
       </c>
-      <c r="E8">
+      <c r="U6">
         <v>100</v>
       </c>
-      <c r="F8">
+      <c r="V6">
         <v>100</v>
       </c>
-      <c r="G8">
+      <c r="W6">
         <v>100</v>
       </c>
-      <c r="H8">
+      <c r="X6">
         <v>100</v>
       </c>
-      <c r="I8" t="s">
+      <c r="Y6" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="8">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Novas telas e ajustes
</commit_message>
<xml_diff>
--- a/Programa/Documentos/1-Análise Primária/Entidades.xlsx
+++ b/Programa/Documentos/1-Análise Primária/Entidades.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
     <sheet name="Pessoa" sheetId="2" r:id="rId2"/>
     <sheet name="Refeição" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -675,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1422,7 +1423,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1683,4 +1684,16 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste de MVVM e implementação de tela de Alimentos
</commit_message>
<xml_diff>
--- a/Programa/Documentos/1-Análise Primária/Entidades.xlsx
+++ b/Programa/Documentos/1-Análise Primária/Entidades.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
   <si>
     <t>Nome</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Frutas, Legumes, Verduras, Carnes, dentre outros</t>
   </si>
   <si>
-    <t>Classe</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -221,13 +218,22 @@
   </si>
   <si>
     <t>TargetWeight</t>
+  </si>
+  <si>
+    <t>Weight Type</t>
+  </si>
+  <si>
+    <t>Tipo de Medição de Peso</t>
+  </si>
+  <si>
+    <t>Gramas, Kilogramas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +401,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -473,6 +484,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -507,6 +519,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -682,26 +695,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="6" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
-    <col min="11" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
     <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -712,7 +725,7 @@
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -732,7 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -774,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -816,36 +829,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
@@ -858,36 +865,18 @@
         <v>27</v>
       </c>
       <c r="R5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S5">
-        <v>100</v>
-      </c>
-      <c r="T5">
-        <v>100</v>
-      </c>
-      <c r="U5">
-        <v>100</v>
-      </c>
-      <c r="V5">
-        <v>100</v>
-      </c>
-      <c r="W5">
-        <v>100</v>
-      </c>
-      <c r="X5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="Y5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
@@ -900,7 +889,7 @@
         <v>27</v>
       </c>
       <c r="R6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="S6">
         <v>100</v>
@@ -921,15 +910,15 @@
         <v>100</v>
       </c>
       <c r="Y6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
@@ -941,13 +930,37 @@
       <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="R7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+      <c r="T7">
+        <v>100</v>
+      </c>
+      <c r="U7">
+        <v>100</v>
+      </c>
+      <c r="V7">
+        <v>100</v>
+      </c>
+      <c r="W7">
+        <v>100</v>
+      </c>
+      <c r="X7">
+        <v>100</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
@@ -960,49 +973,59 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="A10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1010,7 +1033,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1018,7 +1041,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1026,7 +1049,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1034,7 +1057,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1042,7 +1065,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1050,7 +1073,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1058,7 +1081,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1066,7 +1089,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1074,7 +1097,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1082,7 +1105,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1090,7 +1113,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1098,7 +1121,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1106,7 +1129,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1114,13 +1137,21 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1129,21 +1160,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1181,32 +1212,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
@@ -1215,23 +1246,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1249,12 +1280,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
@@ -1267,12 +1298,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
@@ -1285,7 +1316,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1293,7 +1324,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1301,57 +1332,57 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1359,7 +1390,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1367,7 +1398,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1375,7 +1406,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1383,7 +1414,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1391,7 +1422,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1399,7 +1430,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1407,7 +1438,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1415,7 +1446,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1423,7 +1454,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1431,7 +1462,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1439,7 +1470,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1454,14 +1485,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1469,7 +1500,7 @@
     <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1489,13 +1520,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="8">
         <v>6</v>
@@ -1504,16 +1535,16 @@
         <v>23</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -1522,13 +1553,13 @@
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1536,10 +1567,10 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1547,7 +1578,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1555,7 +1586,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1563,7 +1594,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1571,7 +1602,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1579,7 +1610,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
@@ -1587,7 +1618,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1595,7 +1626,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1603,7 +1634,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1611,7 +1642,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1619,7 +1650,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1627,7 +1658,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1635,7 +1666,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1643,7 +1674,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1651,7 +1682,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1659,7 +1690,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1667,7 +1698,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1675,7 +1706,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1683,7 +1714,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1691,7 +1722,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1699,7 +1730,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1707,7 +1738,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1722,12 +1753,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Migrando de Linq to SQL para Entity Framework
</commit_message>
<xml_diff>
--- a/Programa/Documentos/1-Análise Primária/Entidades.xlsx
+++ b/Programa/Documentos/1-Análise Primária/Entidades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>Nome</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Peso objetivado</t>
   </si>
   <si>
-    <t>Pontos por dia</t>
-  </si>
-  <si>
     <t>Pontos extras por semana</t>
   </si>
   <si>
@@ -227,6 +224,18 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>PointsPerDay</t>
+  </si>
+  <si>
+    <t>Pontos Por dia</t>
+  </si>
+  <si>
+    <t>Informa quantos pontos a pessoa pode comer por dia, em alimentos.</t>
+  </si>
+  <si>
+    <t>Int16</t>
   </si>
 </sst>
 </file>
@@ -796,7 +805,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -805,10 +814,10 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
@@ -863,16 +872,16 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
@@ -1162,14 +1171,14 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1">
@@ -1212,14 +1221,14 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
@@ -1228,14 +1237,14 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -1296,7 +1305,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>48</v>
@@ -1313,12 +1322,24 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
@@ -1330,9 +1351,6 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1340,9 +1358,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1350,9 +1366,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1360,8 +1374,8 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1371,7 +1385,7 @@
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1519,10 +1533,10 @@
     <row r="2" spans="1:6">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="8">
         <v>6</v>
@@ -1531,16 +1545,16 @@
         <v>23</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -1549,13 +1563,13 @@
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1563,7 +1577,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6">

</xml_diff>